<commit_message>
Updated TC5 results Rev E
</commit_message>
<xml_diff>
--- a/Test Case - 5/TC5_Results_E.xlsx
+++ b/Test Case - 5/TC5_Results_E.xlsx
@@ -1070,17 +1070,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1088,7 +1086,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1653,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R110" sqref="R110"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1663,46 +1663,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="9" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="10" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="2" t="s">
         <v>126</v>
       </c>
@@ -1721,16 +1721,16 @@
       <c r="G2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="11" t="s">
+      <c r="H2" s="11"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="10" t="s">
         <v>124</v>
       </c>
     </row>
@@ -7161,17 +7161,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="N1:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="M3:M110">
     <cfRule type="cellIs" dxfId="23" priority="47" operator="equal">
@@ -7262,7 +7262,7 @@
   <dimension ref="A1:AA122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7273,50 +7273,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="9" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>134</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11" t="s">
+      <c r="M1" s="10"/>
+      <c r="N1" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11" t="s">
+      <c r="O1" s="10"/>
+      <c r="P1" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11" t="s">
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="S1" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="15" t="s">
         <v>141</v>
       </c>
       <c r="V1" s="3"/>
@@ -7324,7 +7324,7 @@
       <c r="AA1"/>
     </row>
     <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="2" t="s">
         <v>126</v>
       </c>
@@ -7343,19 +7343,19 @@
       <c r="G2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="10"/>
       <c r="J2" s="14"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="12"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="15"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="AA2"/>
@@ -10679,10 +10679,10 @@
         <v>10.0853105804721</v>
       </c>
       <c r="K52" s="2">
-        <v>12.005231732000899</v>
+        <v>10.101378546253599</v>
       </c>
       <c r="L52" s="2">
-        <v>5.2066120410180003</v>
+        <v>4.3809199475601899</v>
       </c>
       <c r="M52" s="2" t="s">
         <v>130</v>
@@ -10705,7 +10705,7 @@
       </c>
       <c r="S52" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T52" t="b">
         <f t="shared" si="3"/>
@@ -10750,10 +10750,10 @@
         <v>10.0853105804721</v>
       </c>
       <c r="K53" s="2">
-        <v>12.005231732000899</v>
+        <v>10.101378546253599</v>
       </c>
       <c r="L53" s="2">
-        <v>5.2066120410180003</v>
+        <v>4.3809199475601899</v>
       </c>
       <c r="M53" s="2" t="s">
         <v>130</v>
@@ -10776,7 +10776,7 @@
       </c>
       <c r="S53" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T53" t="b">
         <f t="shared" si="3"/>
@@ -10821,10 +10821,10 @@
         <v>10.0853105804721</v>
       </c>
       <c r="K54" s="2">
-        <v>12.005231732000899</v>
+        <v>10.101378546253599</v>
       </c>
       <c r="L54" s="2">
-        <v>5.2066120410180003</v>
+        <v>4.3809199475601899</v>
       </c>
       <c r="M54" s="2" t="s">
         <v>130</v>
@@ -10847,7 +10847,7 @@
       </c>
       <c r="S54" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T54" t="b">
         <f t="shared" si="3"/>
@@ -10892,10 +10892,10 @@
         <v>10.0853105804721</v>
       </c>
       <c r="K55" s="2">
-        <v>12.005231732000899</v>
+        <v>10.101378546253599</v>
       </c>
       <c r="L55" s="2">
-        <v>5.2066120410180003</v>
+        <v>4.3809199475601899</v>
       </c>
       <c r="M55" s="2" t="s">
         <v>130</v>
@@ -10918,7 +10918,7 @@
       </c>
       <c r="S55" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T55" t="b">
         <f t="shared" si="3"/>
@@ -11034,10 +11034,10 @@
         <v>10.0853105804721</v>
       </c>
       <c r="K57" s="2">
-        <v>12.005231732000899</v>
+        <v>10.101378546253599</v>
       </c>
       <c r="L57" s="2">
-        <v>5.2066120410180003</v>
+        <v>4.3809199475601899</v>
       </c>
       <c r="M57" s="2" t="s">
         <v>130</v>
@@ -11060,7 +11060,7 @@
       </c>
       <c r="S57" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T57" t="b">
         <f t="shared" si="3"/>
@@ -11105,10 +11105,10 @@
         <v>10.0853105804721</v>
       </c>
       <c r="K58" s="2">
-        <v>12.005231732000899</v>
+        <v>10.101378546253599</v>
       </c>
       <c r="L58" s="2">
-        <v>5.2066120410180003</v>
+        <v>4.3809199475601899</v>
       </c>
       <c r="M58" s="2" t="s">
         <v>130</v>
@@ -11131,7 +11131,7 @@
       </c>
       <c r="S58" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T58" t="b">
         <f t="shared" si="3"/>
@@ -11247,10 +11247,10 @@
         <v>10.0853105804721</v>
       </c>
       <c r="K60" s="2">
-        <v>12.005231732000899</v>
+        <v>10.101378546253599</v>
       </c>
       <c r="L60" s="2">
-        <v>5.2066120410180003</v>
+        <v>4.3809199475601899</v>
       </c>
       <c r="M60" s="2" t="s">
         <v>130</v>
@@ -11273,7 +11273,7 @@
       </c>
       <c r="S60" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T60" t="b">
         <f t="shared" si="3"/>
@@ -11318,10 +11318,10 @@
         <v>10.0853105804721</v>
       </c>
       <c r="K61" s="2">
-        <v>12.005231732000899</v>
+        <v>10.101378546253599</v>
       </c>
       <c r="L61" s="2">
-        <v>5.2066120410180003</v>
+        <v>4.3809199475601899</v>
       </c>
       <c r="M61" s="2" t="s">
         <v>130</v>
@@ -11344,7 +11344,7 @@
       </c>
       <c r="S61" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T61" t="b">
         <f t="shared" si="3"/>
@@ -11389,10 +11389,10 @@
         <v>10.0853105804721</v>
       </c>
       <c r="K62" s="2">
-        <v>12.005231732000899</v>
+        <v>10.101378546253599</v>
       </c>
       <c r="L62" s="2">
-        <v>5.2066120410180003</v>
+        <v>4.3809199475601899</v>
       </c>
       <c r="M62" s="2" t="s">
         <v>130</v>
@@ -11415,7 +11415,7 @@
       </c>
       <c r="S62" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T62" t="b">
         <f t="shared" si="3"/>
@@ -11460,10 +11460,10 @@
         <v>10.0853105804721</v>
       </c>
       <c r="K63" s="2">
-        <v>12.005231732000899</v>
+        <v>10.101378546253599</v>
       </c>
       <c r="L63" s="2">
-        <v>5.2066120410180003</v>
+        <v>4.3809199475601899</v>
       </c>
       <c r="M63" s="2" t="s">
         <v>130</v>
@@ -11486,7 +11486,7 @@
       </c>
       <c r="S63" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T63" t="b">
         <f t="shared" si="3"/>
@@ -11602,10 +11602,10 @@
         <v>10.0853105804721</v>
       </c>
       <c r="K65" s="2">
-        <v>12.005231732000899</v>
+        <v>10.101378546253599</v>
       </c>
       <c r="L65" s="2">
-        <v>5.2066120410180003</v>
+        <v>4.3809199475601899</v>
       </c>
       <c r="M65" s="2" t="s">
         <v>130</v>
@@ -11628,7 +11628,7 @@
       </c>
       <c r="S65" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T65" t="b">
         <f t="shared" si="3"/>
@@ -11673,10 +11673,10 @@
         <v>10.0853105804721</v>
       </c>
       <c r="K66" s="2">
-        <v>12.005231732000899</v>
+        <v>10.101378546253599</v>
       </c>
       <c r="L66" s="2">
-        <v>5.2066120410180003</v>
+        <v>4.3809199475601899</v>
       </c>
       <c r="M66" s="2" t="s">
         <v>130</v>
@@ -11699,7 +11699,7 @@
       </c>
       <c r="S66" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T66" t="b">
         <f t="shared" si="3"/>
@@ -11744,10 +11744,10 @@
         <v>12.7031626622224</v>
       </c>
       <c r="K67" s="2">
-        <v>10.583106496421699</v>
+        <v>12.712999253217401</v>
       </c>
       <c r="L67" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3800647022358303</v>
       </c>
       <c r="M67" s="2" t="s">
         <v>130</v>
@@ -11770,11 +11770,11 @@
       </c>
       <c r="S67" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T67" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U67" s="2" t="s">
         <v>143</v>
@@ -11886,10 +11886,10 @@
         <v>12.7031626622224</v>
       </c>
       <c r="K69" s="2">
-        <v>10.583106496421699</v>
+        <v>12.712999253217401</v>
       </c>
       <c r="L69" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3800647022358303</v>
       </c>
       <c r="M69" s="2" t="s">
         <v>130</v>
@@ -11912,11 +11912,11 @@
       </c>
       <c r="S69" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T69" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U69" s="2" t="s">
         <v>143</v>
@@ -12028,10 +12028,10 @@
         <v>12.7086193526413</v>
       </c>
       <c r="K71" s="2">
-        <v>10.5876525088878</v>
+        <v>12.7086193526413</v>
       </c>
       <c r="L71" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3751281734319099</v>
       </c>
       <c r="M71" s="2" t="s">
         <v>130</v>
@@ -12054,11 +12054,11 @@
       </c>
       <c r="S71" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T71" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U71" s="2" t="s">
         <v>142</v>
@@ -12099,10 +12099,10 @@
         <v>12.7031626622224</v>
       </c>
       <c r="K72" s="2">
-        <v>10.583106496421699</v>
+        <v>12.712999253217401</v>
       </c>
       <c r="L72" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3800647022358303</v>
       </c>
       <c r="M72" s="2" t="s">
         <v>130</v>
@@ -12125,11 +12125,11 @@
       </c>
       <c r="S72" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T72" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U72" s="2" t="s">
         <v>143</v>
@@ -12170,10 +12170,10 @@
         <v>12.7086193526413</v>
       </c>
       <c r="K73" s="2">
-        <v>10.5876525088878</v>
+        <v>12.7086193526413</v>
       </c>
       <c r="L73" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3751281734319099</v>
       </c>
       <c r="M73" s="2" t="s">
         <v>130</v>
@@ -12196,11 +12196,11 @@
       </c>
       <c r="S73" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T73" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U73" s="2" t="s">
         <v>142</v>
@@ -12312,10 +12312,10 @@
         <v>12.7031626622224</v>
       </c>
       <c r="K75" s="2">
-        <v>10.583106496421699</v>
+        <v>12.712999253217401</v>
       </c>
       <c r="L75" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3800647022358303</v>
       </c>
       <c r="M75" s="2" t="s">
         <v>130</v>
@@ -12338,11 +12338,11 @@
       </c>
       <c r="S75" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T75" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U75" s="2" t="s">
         <v>143</v>
@@ -12454,10 +12454,10 @@
         <v>12.7031626622224</v>
       </c>
       <c r="K77" s="2">
-        <v>10.583106496421699</v>
+        <v>12.712999253217401</v>
       </c>
       <c r="L77" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3800647022358303</v>
       </c>
       <c r="M77" s="2" t="s">
         <v>130</v>
@@ -12480,11 +12480,11 @@
       </c>
       <c r="S77" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T77" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U77" s="2" t="s">
         <v>143</v>
@@ -12525,10 +12525,10 @@
         <v>12.7031626622224</v>
       </c>
       <c r="K78" s="2">
-        <v>10.583106496421699</v>
+        <v>12.712999253217401</v>
       </c>
       <c r="L78" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3800647022358303</v>
       </c>
       <c r="M78" s="2" t="s">
         <v>130</v>
@@ -12551,11 +12551,11 @@
       </c>
       <c r="S78" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T78" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U78" s="2" t="s">
         <v>143</v>
@@ -12667,10 +12667,10 @@
         <v>12.7031626622224</v>
       </c>
       <c r="K80" s="2">
-        <v>10.583106496421699</v>
+        <v>12.712999253217401</v>
       </c>
       <c r="L80" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3800647022358303</v>
       </c>
       <c r="M80" s="2" t="s">
         <v>130</v>
@@ -12693,11 +12693,11 @@
       </c>
       <c r="S80" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T80" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U80" s="2" t="s">
         <v>143</v>
@@ -12809,10 +12809,10 @@
         <v>12.7086193526413</v>
       </c>
       <c r="K82" s="2">
-        <v>10.5876525088878</v>
+        <v>12.7086193526413</v>
       </c>
       <c r="L82" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3751281734319099</v>
       </c>
       <c r="M82" s="2" t="s">
         <v>130</v>
@@ -12835,11 +12835,11 @@
       </c>
       <c r="S82" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T82" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U82" s="2" t="s">
         <v>142</v>
@@ -12880,10 +12880,10 @@
         <v>12.7031626622224</v>
       </c>
       <c r="K83" s="2">
-        <v>10.583106496421699</v>
+        <v>12.712999253217401</v>
       </c>
       <c r="L83" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3800647022358303</v>
       </c>
       <c r="M83" s="2" t="s">
         <v>130</v>
@@ -12906,11 +12906,11 @@
       </c>
       <c r="S83" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T83" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U83" s="2" t="s">
         <v>143</v>
@@ -12951,10 +12951,10 @@
         <v>12.7086193526413</v>
       </c>
       <c r="K84" s="2">
-        <v>10.5876525088878</v>
+        <v>12.7086193526413</v>
       </c>
       <c r="L84" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3751281734319099</v>
       </c>
       <c r="M84" s="2" t="s">
         <v>130</v>
@@ -12977,11 +12977,11 @@
       </c>
       <c r="S84" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T84" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U84" s="2" t="s">
         <v>142</v>
@@ -13093,10 +13093,10 @@
         <v>12.7031626622224</v>
       </c>
       <c r="K86" s="2">
-        <v>10.583106496421699</v>
+        <v>12.712999253217401</v>
       </c>
       <c r="L86" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3800647022358303</v>
       </c>
       <c r="M86" s="2" t="s">
         <v>130</v>
@@ -13119,11 +13119,11 @@
       </c>
       <c r="S86" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T86" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U86" s="2" t="s">
         <v>143</v>
@@ -13235,10 +13235,10 @@
         <v>12.7031626622224</v>
       </c>
       <c r="K88" s="2">
-        <v>10.583106496421699</v>
+        <v>12.712999253217401</v>
       </c>
       <c r="L88" s="2">
-        <v>5.3111703110290698</v>
+        <v>6.3800647022358303</v>
       </c>
       <c r="M88" s="2" t="s">
         <v>130</v>
@@ -13261,11 +13261,11 @@
       </c>
       <c r="S88" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T88" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U88" s="2" t="s">
         <v>143</v>
@@ -13377,10 +13377,10 @@
         <v>14.990997475539499</v>
       </c>
       <c r="K90" s="2">
-        <v>9.3519892890220095</v>
+        <v>14.997673134115701</v>
       </c>
       <c r="L90" s="2">
-        <v>5.6092682076984204</v>
+        <v>8.9955161945492392</v>
       </c>
       <c r="M90" s="2" t="s">
         <v>130</v>
@@ -13403,7 +13403,7 @@
       </c>
       <c r="S90" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T90" t="b">
         <f t="shared" si="6"/>
@@ -13448,10 +13448,10 @@
         <v>14.990997475539499</v>
       </c>
       <c r="K91" s="2">
-        <v>9.3519892890220095</v>
+        <v>14.997673134115701</v>
       </c>
       <c r="L91" s="2">
-        <v>5.6092682076984204</v>
+        <v>8.9955161945492392</v>
       </c>
       <c r="M91" s="2" t="s">
         <v>130</v>
@@ -13474,7 +13474,7 @@
       </c>
       <c r="S91" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T91" t="b">
         <f t="shared" si="6"/>
@@ -13519,10 +13519,10 @@
         <v>14.990997475539499</v>
       </c>
       <c r="K92" s="2">
-        <v>9.3519892890220095</v>
+        <v>14.997673134115701</v>
       </c>
       <c r="L92" s="2">
-        <v>5.6092682076984204</v>
+        <v>8.9955161945492392</v>
       </c>
       <c r="M92" s="2" t="s">
         <v>130</v>
@@ -13545,11 +13545,11 @@
       </c>
       <c r="S92" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T92" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U92" s="2" t="s">
         <v>142</v>
@@ -13590,10 +13590,10 @@
         <v>14.990997475539499</v>
       </c>
       <c r="K93" s="2">
-        <v>9.3519892890220095</v>
+        <v>14.997673134115701</v>
       </c>
       <c r="L93" s="2">
-        <v>5.6092682076984204</v>
+        <v>8.9955161945492392</v>
       </c>
       <c r="M93" s="2" t="s">
         <v>130</v>
@@ -13616,7 +13616,7 @@
       </c>
       <c r="S93" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T93" t="b">
         <f t="shared" si="6"/>
@@ -13661,10 +13661,10 @@
         <v>14.990997475539499</v>
       </c>
       <c r="K94" s="2">
-        <v>9.3519892890220095</v>
+        <v>14.997673134115701</v>
       </c>
       <c r="L94" s="2">
-        <v>5.6092682076984204</v>
+        <v>8.9955161945492392</v>
       </c>
       <c r="M94" s="2" t="s">
         <v>130</v>
@@ -13687,7 +13687,7 @@
       </c>
       <c r="S94" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T94" t="b">
         <f t="shared" si="6"/>
@@ -13732,10 +13732,10 @@
         <v>14.990997475539499</v>
       </c>
       <c r="K95" s="2">
-        <v>9.3519892890220095</v>
+        <v>14.997673134115701</v>
       </c>
       <c r="L95" s="2">
-        <v>5.6092682076984204</v>
+        <v>8.9955161945492392</v>
       </c>
       <c r="M95" s="2" t="s">
         <v>130</v>
@@ -13758,11 +13758,11 @@
       </c>
       <c r="S95" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T95" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U95" s="2" t="s">
         <v>142</v>
@@ -13803,10 +13803,10 @@
         <v>14.990997475539499</v>
       </c>
       <c r="K96" s="2">
-        <v>9.3519892890220095</v>
+        <v>14.997673134115701</v>
       </c>
       <c r="L96" s="2">
-        <v>5.6092682076984204</v>
+        <v>8.9955161945492392</v>
       </c>
       <c r="M96" s="2" t="s">
         <v>130</v>
@@ -13829,7 +13829,7 @@
       </c>
       <c r="S96" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T96" t="b">
         <f t="shared" si="6"/>
@@ -13874,10 +13874,10 @@
         <v>14.990997475539499</v>
       </c>
       <c r="K97" s="2">
-        <v>9.3519892890220095</v>
+        <v>14.997673134115701</v>
       </c>
       <c r="L97" s="2">
-        <v>5.6092682076984204</v>
+        <v>8.9955161945492392</v>
       </c>
       <c r="M97" s="2" t="s">
         <v>130</v>
@@ -13900,7 +13900,7 @@
       </c>
       <c r="S97" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T97" t="b">
         <f t="shared" si="6"/>
@@ -14016,10 +14016,10 @@
         <v>14.990997475539499</v>
       </c>
       <c r="K99" s="2">
-        <v>9.3519892890220095</v>
+        <v>14.997673134115701</v>
       </c>
       <c r="L99" s="2">
-        <v>5.6092682076984204</v>
+        <v>8.9955161945492392</v>
       </c>
       <c r="M99" s="2" t="s">
         <v>130</v>
@@ -14042,7 +14042,7 @@
       </c>
       <c r="S99" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T99" t="b">
         <f t="shared" si="6"/>
@@ -14087,10 +14087,10 @@
         <v>14.990997475539499</v>
       </c>
       <c r="K100" s="2">
-        <v>9.3519892890220095</v>
+        <v>14.997673134115701</v>
       </c>
       <c r="L100" s="2">
-        <v>5.6092682076984204</v>
+        <v>8.9955161945492392</v>
       </c>
       <c r="M100" s="2" t="s">
         <v>130</v>
@@ -14113,7 +14113,7 @@
       </c>
       <c r="S100" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T100" t="b">
         <f t="shared" si="6"/>
@@ -14229,10 +14229,10 @@
         <v>16.7511617101915</v>
       </c>
       <c r="K102" s="2">
-        <v>8.9451565179695702</v>
+        <v>16.756755326080299</v>
       </c>
       <c r="L102" s="2">
-        <v>5.8534464843330296</v>
+        <v>10.965126250752</v>
       </c>
       <c r="M102" s="2" t="s">
         <v>130</v>
@@ -14255,7 +14255,7 @@
       </c>
       <c r="S102" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T102" t="b">
         <f t="shared" si="6"/>
@@ -14371,10 +14371,10 @@
         <v>16.7511617101915</v>
       </c>
       <c r="K104" s="2">
-        <v>8.9451565179695702</v>
+        <v>16.756755326080299</v>
       </c>
       <c r="L104" s="2">
-        <v>5.8534464843330296</v>
+        <v>10.965126250752</v>
       </c>
       <c r="M104" s="2" t="s">
         <v>130</v>
@@ -14397,7 +14397,7 @@
       </c>
       <c r="S104" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T104" t="b">
         <f t="shared" si="6"/>
@@ -14442,10 +14442,10 @@
         <v>16.7511617101915</v>
       </c>
       <c r="K105" s="2">
-        <v>8.9451565179695702</v>
+        <v>16.756755326080299</v>
       </c>
       <c r="L105" s="2">
-        <v>5.8534464843330296</v>
+        <v>10.965126250752</v>
       </c>
       <c r="M105" s="2" t="s">
         <v>130</v>
@@ -14468,7 +14468,7 @@
       </c>
       <c r="S105" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T105" t="b">
         <f t="shared" si="6"/>
@@ -14584,10 +14584,10 @@
         <v>16.7511617101915</v>
       </c>
       <c r="K107" s="2">
-        <v>8.9451565179695702</v>
+        <v>16.756755326080299</v>
       </c>
       <c r="L107" s="2">
-        <v>5.8534464843330296</v>
+        <v>10.965126250752</v>
       </c>
       <c r="M107" s="2" t="s">
         <v>130</v>
@@ -14610,7 +14610,7 @@
       </c>
       <c r="S107" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T107" t="b">
         <f t="shared" si="6"/>
@@ -14726,10 +14726,10 @@
         <v>16.7511617101915</v>
       </c>
       <c r="K109" s="2">
-        <v>8.9451565179695702</v>
+        <v>16.756755326080299</v>
       </c>
       <c r="L109" s="2">
-        <v>5.8534464843330296</v>
+        <v>10.965126250752</v>
       </c>
       <c r="M109" s="2" t="s">
         <v>130</v>
@@ -14752,7 +14752,7 @@
       </c>
       <c r="S109" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T109" t="b">
         <f t="shared" si="6"/>
@@ -14797,10 +14797,10 @@
         <v>16.7511617101915</v>
       </c>
       <c r="K110" s="2">
-        <v>8.9451565179695702</v>
+        <v>16.756755326080299</v>
       </c>
       <c r="L110" s="2">
-        <v>5.8534464843330296</v>
+        <v>10.965126250752</v>
       </c>
       <c r="M110" s="2" t="s">
         <v>130</v>
@@ -14823,7 +14823,7 @@
       </c>
       <c r="S110" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T110" t="b">
         <f t="shared" si="6"/>
@@ -14939,10 +14939,10 @@
         <v>18.363729223026699</v>
       </c>
       <c r="K112" s="2">
-        <v>9.4358298522203796</v>
+        <v>18.369536607290499</v>
       </c>
       <c r="L112" s="2">
-        <v>6.2675818651956998</v>
+        <v>12.2016374092216</v>
       </c>
       <c r="M112" s="2" t="s">
         <v>130</v>
@@ -14965,7 +14965,7 @@
       </c>
       <c r="S112" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T112" t="b">
         <f t="shared" si="6"/>
@@ -15081,10 +15081,10 @@
         <v>18.363729223026699</v>
       </c>
       <c r="K114" s="2">
-        <v>9.4358298522203796</v>
+        <v>18.369536607290499</v>
       </c>
       <c r="L114" s="2">
-        <v>6.2675818651956998</v>
+        <v>12.2016374092216</v>
       </c>
       <c r="M114" s="2" t="s">
         <v>130</v>
@@ -15107,7 +15107,7 @@
       </c>
       <c r="S114" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T114" t="b">
         <f t="shared" si="6"/>
@@ -15152,10 +15152,10 @@
         <v>18.363729223026699</v>
       </c>
       <c r="K115" s="2">
-        <v>9.4358298522203796</v>
+        <v>18.369536607290499</v>
       </c>
       <c r="L115" s="2">
-        <v>6.2675818651956998</v>
+        <v>12.2016374092216</v>
       </c>
       <c r="M115" s="2" t="s">
         <v>130</v>
@@ -15178,7 +15178,7 @@
       </c>
       <c r="S115" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T115" t="b">
         <f t="shared" si="6"/>
@@ -15294,10 +15294,10 @@
         <v>18.363729223026699</v>
       </c>
       <c r="K117" s="2">
-        <v>9.4358298522203796</v>
+        <v>18.369536607290499</v>
       </c>
       <c r="L117" s="2">
-        <v>6.2675818651956998</v>
+        <v>12.2016374092216</v>
       </c>
       <c r="M117" s="2" t="s">
         <v>130</v>
@@ -15320,7 +15320,7 @@
       </c>
       <c r="S117" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T117" t="b">
         <f t="shared" si="6"/>
@@ -15360,12 +15360,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:M2"/>
@@ -15373,6 +15367,12 @@
     <mergeCell ref="P1:Q2"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="R3:R117 T3:T117 U4:U118">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
@@ -15517,7 +15517,7 @@
       <c r="A6" t="s">
         <v>164</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="9" t="s">
         <v>165</v>
       </c>
       <c r="C6" t="s">

</xml_diff>